<commit_message>
Adjust ARpUIiRC and edit to SoCEUtiNTY
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Component Lifetimes" sheetId="3" r:id="rId2"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -588,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD26"/>
     </sheetView>
   </sheetViews>
@@ -773,8 +773,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -868,16 +868,15 @@
         <v>7</v>
       </c>
       <c r="B6" s="9">
-        <f>1/'Component Lifetimes'!B6</f>
-        <v>8.6956521739130432E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C6" s="4">
         <f>B6</f>
-        <v>8.6956521739130432E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
-        <v>8.6956521739130432E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>